<commit_message>
Se completa seccion Security
</commit_message>
<xml_diff>
--- a/reports/Sales-JUNE.xlsx
+++ b/reports/Sales-JUNE.xlsx
@@ -29,10 +29,10 @@
     <t>Ragnar Lothbrok</t>
   </si>
   <si>
-    <t>GOTW771012HMRGR087</t>
+    <t>BBMB771012HMCRR022</t>
   </si>
   <si>
-    <t>Khal Drogo</t>
+    <t>Walter White</t>
   </si>
   <si>
     <t>WALA771012HCRGR054</t>
@@ -41,10 +41,10 @@
     <t>Wednesday Addams</t>
   </si>
   <si>
-    <t>BBMB771012HMCRR022</t>
+    <t>GOTW771012HMRGR087</t>
   </si>
   <si>
-    <t>Walter White</t>
+    <t>Khal Drogo</t>
   </si>
 </sst>
 </file>
@@ -160,7 +160,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n" s="2">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -171,7 +171,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n" s="2">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>